<commit_message>
Add test for sample records with SubjectName longer than 30 characters
</commit_message>
<xml_diff>
--- a/importScripts/rwahsSubjectListMapping.xlsx
+++ b/importScripts/rwahsSubjectListMapping.xlsx
@@ -2229,7 +2229,7 @@
       <c r="L14" s="31"/>
       <c r="M14" s="32" t="str">
         <f>validateJson(E14, G14)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N14" s="33" t="s">
         <v>67</v>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="Y14" s="34" t="str">
         <f>camelToTitle(X14)</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z14" s="33" t="s">
         <v>20</v>
@@ -2304,17 +2304,7 @@
   &lt;/typeRestrictions&gt;
 &lt;/metadataElement&gt;
 ","")</f>
-        <v>&lt;metadataElement code='' datatype='List' list='SubjectType'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_'&gt;
-       &lt;table&gt;&lt;/table&gt;
-       &lt;type&gt;subjectList&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="15">
@@ -2383,7 +2373,7 @@
       <c r="L16" s="31"/>
       <c r="M16" s="32" t="str">
         <f t="shared" ref="M16:M33" si="1">validateJson(E16, G16)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N16" s="33" t="s">
         <v>67</v>
@@ -2479,7 +2469,7 @@
       <c r="L17" s="31"/>
       <c r="M17" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N17" s="33" t="s">
         <v>67</v>
@@ -2525,7 +2515,7 @@
       </c>
       <c r="Y17" s="34" t="str">
         <f t="shared" ref="Y17:Y33" si="6">camelToTitle(X17)</f>
-        <v>Subject Dates</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z17" s="33" t="s">
         <v>78</v>
@@ -2542,17 +2532,7 @@
       </c>
       <c r="AE17" s="36" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;metadataElement code='SubjectDates' datatype='DateRange'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;Subject Dates&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_SubjectDates'&gt;
-       &lt;table&gt;ca_occurrences&lt;/table&gt;
-       &lt;type&gt;subjectList&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="18">
@@ -2578,7 +2558,7 @@
       <c r="L18" s="31"/>
       <c r="M18" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N18" s="33"/>
       <c r="O18" s="33" t="s">
@@ -2622,7 +2602,7 @@
       </c>
       <c r="Y18" s="34" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z18" s="34"/>
       <c r="AA18" s="34"/>
@@ -2637,17 +2617,7 @@
       </c>
       <c r="AE18" s="36" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;metadataElement code='' datatype='Text'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_'&gt;
-       &lt;table&gt;&lt;/table&gt;
-       &lt;type&gt;subjectList&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="19">
@@ -2673,7 +2643,7 @@
       <c r="L19" s="31"/>
       <c r="M19" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N19" s="33" t="s">
         <v>67</v>
@@ -2719,7 +2689,7 @@
       </c>
       <c r="Y19" s="34" t="str">
         <f t="shared" si="6"/>
-        <v>Last Edit By</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z19" s="33" t="s">
         <v>83</v>
@@ -2736,17 +2706,7 @@
       </c>
       <c r="AE19" s="36" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;metadataElement code='LastEditBy' datatype='Text'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;Last Edit By&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_LastEditBy'&gt;
-       &lt;table&gt;ca_occurrences&lt;/table&gt;
-       &lt;type&gt;subjectList&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="20">
@@ -2772,7 +2732,7 @@
       <c r="L20" s="31"/>
       <c r="M20" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N20" s="33" t="s">
         <v>67</v>
@@ -2818,7 +2778,7 @@
       </c>
       <c r="Y20" s="34" t="str">
         <f t="shared" si="6"/>
-        <v>Last Edit Date</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z20" s="33" t="s">
         <v>78</v>
@@ -2835,17 +2795,7 @@
       </c>
       <c r="AE20" s="36" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;metadataElement code='LastEditDate' datatype='DateRange'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;Last Edit Date&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_LastEditDate'&gt;
-       &lt;table&gt;ca_occurrences&lt;/table&gt;
-       &lt;type&gt;subjectList&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="21">
@@ -2871,7 +2821,7 @@
       <c r="L21" s="31"/>
       <c r="M21" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N21" s="33"/>
       <c r="O21" s="33" t="s">
@@ -2915,7 +2865,7 @@
       </c>
       <c r="Y21" s="34" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z21" s="34"/>
       <c r="AA21" s="34"/>
@@ -2930,17 +2880,7 @@
       </c>
       <c r="AE21" s="36" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;metadataElement code='' datatype='Text'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_'&gt;
-       &lt;table&gt;&lt;/table&gt;
-       &lt;type&gt;subjectList&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="22">
@@ -2966,7 +2906,7 @@
       <c r="L22" s="31"/>
       <c r="M22" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N22" s="33" t="s">
         <v>91</v>
@@ -3012,7 +2952,7 @@
       </c>
       <c r="Y22" s="34" t="str">
         <f t="shared" si="6"/>
-        <v>Description</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z22" s="33" t="s">
         <v>83</v>
@@ -3029,17 +2969,7 @@
       </c>
       <c r="AE22" s="36" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;metadataElement code='Description' datatype='Text'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;Description&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_Description'&gt;
-       &lt;table&gt;ca_occurrences&lt;/table&gt;
-       &lt;type&gt;subjectList&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="23">
@@ -3065,7 +2995,7 @@
       <c r="L23" s="31"/>
       <c r="M23" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N23" s="33"/>
       <c r="O23" s="33" t="s">
@@ -3109,7 +3039,7 @@
       </c>
       <c r="Y23" s="34" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z23" s="34"/>
       <c r="AA23" s="34"/>
@@ -3123,17 +3053,7 @@
       </c>
       <c r="AE23" s="36" t="str">
         <f t="shared" si="5"/>
-        <v>&lt;metadataElement code='' datatype='Text'&gt;
-  &lt;labels&gt;&lt;label locale='en_AU'&gt;&lt;name&gt;&lt;/name&gt;&lt;/label&gt;&lt;/labels&gt;
-  &lt;typeRestrictions&gt;
-    &lt;restriction code='museum_'&gt;
-       &lt;table&gt;&lt;/table&gt;
-       &lt;type&gt;subjectList&lt;/type&gt;
-       &lt;includeSubtypes&gt;true&lt;/includeSubtypes&gt;
-    &lt;/restriction&gt;
-  &lt;/typeRestrictions&gt;
-&lt;/metadataElement&gt;
-</v>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="24">
@@ -3157,7 +3077,7 @@
       <c r="L24" s="31"/>
       <c r="M24" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N24" s="33"/>
       <c r="O24" s="33" t="s">
@@ -3201,7 +3121,7 @@
       </c>
       <c r="Y24" s="34" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z24" s="34" t="str">
         <f>VLOOKUP($B24,sampleDataObjects,Z$1,false)</f>
@@ -3249,7 +3169,7 @@
       <c r="L25" s="31"/>
       <c r="M25" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N25" s="33" t="s">
         <v>67</v>
@@ -3295,7 +3215,7 @@
       </c>
       <c r="Y25" s="34" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z25" s="34" t="str">
         <f>VLOOKUP($B25,sampleDataObjects,Z$1,false)</f>
@@ -3338,7 +3258,7 @@
       <c r="L26" s="31"/>
       <c r="M26" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N26" s="33" t="s">
         <v>67</v>
@@ -3384,7 +3304,7 @@
       </c>
       <c r="Y26" s="34" t="str">
         <f t="shared" si="6"/>
-        <v>Association</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z26" s="34" t="str">
         <f>VLOOKUP($B26,sampleDataObjects,Z$1,false)</f>
@@ -3428,7 +3348,7 @@
       <c r="L27" s="31"/>
       <c r="M27" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N27" s="33" t="s">
         <v>67</v>
@@ -3474,7 +3394,7 @@
       </c>
       <c r="Y27" s="34" t="str">
         <f t="shared" si="6"/>
-        <v>Subject Dates</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z27" s="34" t="str">
         <f>VLOOKUP($B27,sampleDataObjects,Z$1,false)</f>
@@ -3518,7 +3438,7 @@
       <c r="L28" s="31"/>
       <c r="M28" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N28" s="33" t="s">
         <v>105</v>
@@ -3564,7 +3484,7 @@
       </c>
       <c r="Y28" s="34" t="str">
         <f t="shared" si="6"/>
-        <v>Sdatetime</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z28" s="34" t="str">
         <f>VLOOKUP($B28,sampleDataObjects,Z$1,false)</f>
@@ -3608,7 +3528,7 @@
       <c r="L29" s="31"/>
       <c r="M29" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N29" s="33" t="s">
         <v>105</v>
@@ -3654,7 +3574,7 @@
       </c>
       <c r="Y29" s="34" t="str">
         <f t="shared" si="6"/>
-        <v>Edatetime</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z29" s="34" t="str">
         <f>VLOOKUP($B29,sampleDataObjects,Z$1,false)</f>
@@ -3698,7 +3618,7 @@
       <c r="L30" s="31"/>
       <c r="M30" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N30" s="33" t="s">
         <v>67</v>
@@ -3744,7 +3664,7 @@
       </c>
       <c r="Y30" s="34" t="str">
         <f t="shared" si="6"/>
-        <v>Type_id</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z30" s="34" t="str">
         <f>VLOOKUP($B30,sampleDataObjects,Z$1,false)</f>
@@ -3788,7 +3708,7 @@
       <c r="L31" s="31"/>
       <c r="M31" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N31" s="33" t="s">
         <v>112</v>
@@ -3834,7 +3754,7 @@
       </c>
       <c r="Y31" s="34" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z31" s="34" t="str">
         <f>VLOOKUP($B31,sampleDataObjects,Z$1,false)</f>
@@ -3876,7 +3796,7 @@
       <c r="L32" s="31"/>
       <c r="M32" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N32" s="43" t="s">
         <v>114</v>
@@ -3922,7 +3842,7 @@
       </c>
       <c r="Y32" s="34" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z32" s="34" t="str">
         <f>VLOOKUP($B32,sampleDataObjects,Z$1,false)</f>
@@ -3970,7 +3890,7 @@
       <c r="L33" s="31"/>
       <c r="M33" s="32" t="str">
         <f t="shared" si="1"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N33" s="33" t="s">
         <v>118</v>
@@ -4016,7 +3936,7 @@
       </c>
       <c r="Y33" s="34" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#NAME?</v>
       </c>
       <c r="Z33" s="34" t="str">
         <f>VLOOKUP($B33,sampleDataObjects,Z$1,false)</f>
@@ -4097,7 +4017,7 @@
       <c r="L35" s="31"/>
       <c r="M35" s="32" t="str">
         <f t="shared" ref="M35:M39" si="8">validateJson(E35, G35)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N35" s="33" t="s">
         <v>112</v>
@@ -4143,7 +4063,7 @@
       </c>
       <c r="Y35" s="34" t="str">
         <f t="shared" ref="Y35:Y39" si="12">camelToTitle(X35)</f>
-        <v>Association</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z35" s="34" t="str">
         <f>VLOOKUP($B35,sampleDataObjects,Z$1,false)</f>
@@ -4195,7 +4115,7 @@
       <c r="L36" s="31"/>
       <c r="M36" s="32" t="str">
         <f t="shared" si="8"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N36" s="33" t="s">
         <v>91</v>
@@ -4241,7 +4161,7 @@
       </c>
       <c r="Y36" s="34" t="str">
         <f t="shared" si="12"/>
-        <v>Subject Dates</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z36" s="34" t="str">
         <f>VLOOKUP($B36,sampleDataObjects,Z$1,false)</f>
@@ -4283,7 +4203,7 @@
       <c r="L37" s="31"/>
       <c r="M37" s="32" t="str">
         <f t="shared" si="8"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N37" s="33" t="s">
         <v>105</v>
@@ -4329,7 +4249,7 @@
       </c>
       <c r="Y37" s="34" t="str">
         <f t="shared" si="12"/>
-        <v>Sdatetime</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z37" s="34" t="str">
         <f>VLOOKUP($B37,sampleDataObjects,Z$1,false)</f>
@@ -4371,7 +4291,7 @@
       <c r="L38" s="31"/>
       <c r="M38" s="32" t="str">
         <f t="shared" si="8"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N38" s="33" t="s">
         <v>105</v>
@@ -4417,7 +4337,7 @@
       </c>
       <c r="Y38" s="34" t="str">
         <f t="shared" si="12"/>
-        <v>Edatetime</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z38" s="34" t="str">
         <f>VLOOKUP($B38,sampleDataObjects,Z$1,false)</f>
@@ -4459,7 +4379,7 @@
       <c r="L39" s="31"/>
       <c r="M39" s="32" t="str">
         <f t="shared" si="8"/>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N39" s="33" t="s">
         <v>118</v>
@@ -4505,7 +4425,7 @@
       </c>
       <c r="Y39" s="34" t="str">
         <f t="shared" si="12"/>
-        <v>Type_id</v>
+        <v>#NAME?</v>
       </c>
       <c r="Z39" s="34" t="str">
         <f>VLOOKUP($B39,sampleDataObjects,Z$1,false)</f>
@@ -4654,7 +4574,7 @@
       <c r="L43" s="31"/>
       <c r="M43" s="32" t="str">
         <f>validateJson(E43, G43)</f>
-        <v>TRUE</v>
+        <v>#NAME?</v>
       </c>
       <c r="N43" s="33"/>
       <c r="O43" s="33" t="s">

</xml_diff>